<commit_message>
inlineForeignTabs 可编辑聚合表格, isDeleteCascade 级联删除
</commit_message>
<xml_diff>
--- a/codegen/__out__/pc/public/excel_template/base/dict_detail.xlsx
+++ b/codegen/__out__/pc/public/excel_template/base/dict_detail.xlsx
@@ -51,6 +51,18 @@
     <t xml:space="preserve">&lt;%=comment.rem%&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;%=comment.create_usr_id_lbl%&gt;&lt;%selectList.create_usr_id = data.findAllUsr.map((item) =&gt; item.lbl)%&gt;&lt;%_dataValidation_({ sqref: `${ _col }2:${ _col }${ _lastRow }`, formula1: `"${ selectList.create_usr_id.join(",") }"` })%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%=comment.create_time_lbl%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%=comment.update_usr_id_lbl%&gt;&lt;%selectList.update_usr_id = data.findAllUsr.map((item) =&gt; item.lbl)%&gt;&lt;%_dataValidation_({ sqref: `${ _col }2:${ _col }${ _lastRow }`, formula1: `"${ selectList.update_usr_id.join(",") }"` })%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%=comment.update_time_lbl%&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;%forRow model in data.findAllDictDetail%&gt;&lt;%=model.dict_id_lbl%&gt;</t>
   </si>
   <si>
@@ -70,6 +82,18 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;%=model.rem%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%=model.create_usr_id_lbl%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%~model.create_time ? new Date(model.create_time) : ""%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%=model.update_usr_id_lbl%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%~model.update_time ? new Date(model.update_time) : ""%&gt;</t>
   </si>
 </sst>
 </file>
@@ -422,28 +446,52 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>